<commit_message>
updated cohensKappaCalculator to support 3 + 4 class cases
</commit_message>
<xml_diff>
--- a/analytics/cohensKappaCalculator.xlsx
+++ b/analytics/cohensKappaCalculator.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\Business\Work\University\Degree - Masters\3a - Thesis\code\analytics\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39F28BF-8B7C-4C1D-BB56-64A8FAF7D3FD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="3120" windowWidth="10960" windowHeight="7000" tabRatio="500"/>
+    <workbookView xWindow="420" yWindow="3720" windowWidth="10965" windowHeight="7005" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="179017" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="11">
   <si>
     <t>TRUTH</t>
   </si>
@@ -40,12 +46,24 @@
   </si>
   <si>
     <t>Class B</t>
+  </si>
+  <si>
+    <t>Class C</t>
+  </si>
+  <si>
+    <t>Class D</t>
+  </si>
+  <si>
+    <t>col total</t>
+  </si>
+  <si>
+    <t>row total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -110,6 +128,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -434,21 +460,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A2:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>5</v>
       </c>
@@ -456,7 +482,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>1</v>
       </c>
@@ -477,7 +503,7 @@
         <v>0.57999999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>6</v>
       </c>
@@ -495,13 +521,265 @@
         <v>0.49199999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>4</v>
       </c>
       <c r="G6">
         <f>(G4-G5)/(1-G5)</f>
         <v>0.17322834645669286</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <f>SUM(C12:E12)</f>
+        <v>1</v>
+      </c>
+      <c r="H12" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <f>(C12+D13+E14)/F15</f>
+        <v>0.52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>18</v>
+      </c>
+      <c r="E13">
+        <v>10</v>
+      </c>
+      <c r="F13">
+        <f>SUM(C13:E13)</f>
+        <v>29</v>
+      </c>
+      <c r="H13" t="s">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <f>(C15*F12 + D15*F13+E15*F14)/(F15^2)</f>
+        <v>0.49640000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>13</v>
+      </c>
+      <c r="E14">
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <f>SUM(C14:E14)</f>
+        <v>20</v>
+      </c>
+      <c r="H14" t="s">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <f>(I12-I13)/(1-I13)</f>
+        <v>4.6862589356632262E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15">
+        <f>SUM(C12:C14)</f>
+        <v>2</v>
+      </c>
+      <c r="D15">
+        <f>SUM(D12:D14)</f>
+        <v>31</v>
+      </c>
+      <c r="E15">
+        <f>SUM(E12:E14)</f>
+        <v>17</v>
+      </c>
+      <c r="F15">
+        <f>IF(SUM(F12:F14)=SUM(C15:E15),SUM(C15:E15),CONCATENATE("R=",SUM(C15:E15),", C=",SUM(F12:F14)))</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="C20" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>7</v>
+      </c>
+      <c r="F20" t="s">
+        <v>8</v>
+      </c>
+      <c r="G20" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <f>SUM(C21:F21)</f>
+        <v>0</v>
+      </c>
+      <c r="I21" t="s">
+        <v>2</v>
+      </c>
+      <c r="J21">
+        <f>(C21+D22+E23+F24)/G25</f>
+        <v>0.63888888888888884</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22">
+        <v>9</v>
+      </c>
+      <c r="E22">
+        <v>3</v>
+      </c>
+      <c r="F22">
+        <v>1</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ref="G22:G24" si="0">SUM(C22:F22)</f>
+        <v>13</v>
+      </c>
+      <c r="I22" t="s">
+        <v>3</v>
+      </c>
+      <c r="J22">
+        <f>(C25*G21+D25*G22+E25*G23+F25*G24)/(G25^2)</f>
+        <v>0.34259259259259262</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>4</v>
+      </c>
+      <c r="E23">
+        <v>8</v>
+      </c>
+      <c r="F23">
+        <v>2</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="I23" t="s">
+        <v>4</v>
+      </c>
+      <c r="J23">
+        <f>(J21-J22)/(1-J22)</f>
+        <v>0.45070422535211252</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>6</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <f>SUM(C21:C24)</f>
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <f t="shared" ref="D25:F25" si="1">SUM(D21:D24)</f>
+        <v>15</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="F25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G25">
+        <f>IF(SUM(G21:G24)=SUM(C25:F25),SUM(C25:F25),CONCATENATE("R=",SUM(C25:F25),", C=",SUM(G21:G24)))</f>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final upload/last changes for thesis composition
</commit_message>
<xml_diff>
--- a/analytics/cohensKappaCalculator.xlsx
+++ b/analytics/cohensKappaCalculator.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20325"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GoogleDrive\Business\Work\University\Degree - Masters\3a - Thesis\code\analytics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39F28BF-8B7C-4C1D-BB56-64A8FAF7D3FD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C377B367-D167-4C87-8BA2-F1DF8972F94B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="420" yWindow="3720" windowWidth="10965" windowHeight="7005" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="420" yWindow="4320" windowWidth="10965" windowHeight="7005" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Comparison to other Studies" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="179017" concurrentCalc="0"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="12">
   <si>
     <t>TRUTH</t>
   </si>
@@ -58,6 +59,9 @@
   </si>
   <si>
     <t>row total</t>
+  </si>
+  <si>
+    <t>https://ieeexplore.ieee.org/document/6449272/</t>
   </si>
 </sst>
 </file>
@@ -463,8 +467,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:J25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -791,4 +795,151 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8566AAF7-778E-4BC1-A653-9EB4A9A3470D}">
+  <dimension ref="A1:G16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3">
+        <v>28</v>
+      </c>
+      <c r="D3">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <f>(C3+D4)/SUM(C3:D4)</f>
+        <v>0.85365853658536583</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>3</v>
+      </c>
+      <c r="G4">
+        <f>(SUM(C3:C4)*SUM(C3:D3) + SUM(D3:D4)*SUM(C4:D4))/(SUM(C3:D4)^2)</f>
+        <v>0.62998215348007136</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5">
+        <f>(G3-G4)/(1-G4)</f>
+        <v>0.60450160771704176</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12">
+        <v>14</v>
+      </c>
+      <c r="D12">
+        <v>3</v>
+      </c>
+      <c r="F12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12">
+        <f>(C12+D13)/SUM(C12:D13)</f>
+        <v>0.7931034482758621</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13">
+        <v>9</v>
+      </c>
+      <c r="F13" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13">
+        <f>(SUM(C12:C13)*SUM(C12:D12) + SUM(D12:D13)*SUM(C13:D13))/(SUM(C12:D13)^2)</f>
+        <v>0.51486325802615929</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14">
+        <f>(G12-G13)/(1-G13)</f>
+        <v>0.57352941176470595</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>